<commit_message>
factor(controller_factorise): add last multiplefiles or tabs methods
</commit_message>
<xml_diff>
--- a/fichiers_xls/test_merging.xlsx
+++ b/fichiers_xls/test_merging.xlsx
@@ -355,7 +355,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A8:D14"/>
@@ -442,8 +442,13 @@
         <v/>
       </c>
     </row>
+    <row r="12"/>
+    <row r="13"/>
+    <row r="14"/>
+    <row r="15"/>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
+    <mergeCell ref="C12:D15"/>
     <mergeCell ref="C5:D7"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
@@ -466,7 +471,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A8:D14"/>
@@ -572,8 +577,13 @@
         <v/>
       </c>
     </row>
+    <row r="12"/>
+    <row r="13"/>
+    <row r="14"/>
+    <row r="15"/>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
+    <mergeCell ref="C12:D15"/>
     <mergeCell ref="C5:D7"/>
   </mergeCells>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
@@ -596,7 +606,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A5:D10"/>
+  <dimension ref="A5:D15"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8:D14"/>
@@ -621,8 +631,13 @@
         <v/>
       </c>
     </row>
+    <row r="12"/>
+    <row r="13"/>
+    <row r="14"/>
+    <row r="15"/>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
+    <mergeCell ref="C12:D15"/>
     <mergeCell ref="C5:D7"/>
   </mergeCells>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
@@ -645,7 +660,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A5:D10"/>
+  <dimension ref="A5:D15"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="A8:D14"/>
@@ -670,8 +685,13 @@
         <v/>
       </c>
     </row>
+    <row r="12"/>
+    <row r="13"/>
+    <row r="14"/>
+    <row r="15"/>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
+    <mergeCell ref="C12:D15"/>
     <mergeCell ref="C5:D7"/>
   </mergeCells>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
@@ -694,7 +714,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A5:D10"/>
+  <dimension ref="A5:D15"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="A8:D14"/>
@@ -719,8 +739,13 @@
         <v/>
       </c>
     </row>
+    <row r="12"/>
+    <row r="13"/>
+    <row r="14"/>
+    <row r="15"/>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
+    <mergeCell ref="C12:D15"/>
     <mergeCell ref="C5:D7"/>
   </mergeCells>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
@@ -743,7 +768,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A5:D10"/>
+  <dimension ref="A5:D15"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="A8:D14"/>
@@ -768,8 +793,13 @@
         <v/>
       </c>
     </row>
+    <row r="12"/>
+    <row r="13"/>
+    <row r="14"/>
+    <row r="15"/>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
+    <mergeCell ref="C12:D15"/>
     <mergeCell ref="C5:D7"/>
   </mergeCells>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
@@ -792,7 +822,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A5:D10"/>
+  <dimension ref="A5:D15"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="A8:D14"/>
@@ -817,8 +847,13 @@
         <v/>
       </c>
     </row>
+    <row r="12"/>
+    <row r="13"/>
+    <row r="14"/>
+    <row r="15"/>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
+    <mergeCell ref="C12:D15"/>
     <mergeCell ref="C5:D7"/>
   </mergeCells>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
@@ -841,7 +876,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A5:D10"/>
+  <dimension ref="A5:D15"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="A8:D14"/>
@@ -866,8 +901,13 @@
         <v/>
       </c>
     </row>
+    <row r="12"/>
+    <row r="13"/>
+    <row r="14"/>
+    <row r="15"/>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
+    <mergeCell ref="C12:D15"/>
     <mergeCell ref="C5:D7"/>
   </mergeCells>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
@@ -890,7 +930,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A5:D10"/>
+  <dimension ref="A5:D15"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="A8:D14"/>
@@ -915,8 +955,13 @@
         <v/>
       </c>
     </row>
+    <row r="12"/>
+    <row r="13"/>
+    <row r="14"/>
+    <row r="15"/>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
+    <mergeCell ref="C12:D15"/>
     <mergeCell ref="C5:D7"/>
   </mergeCells>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>

</xml_diff>